<commit_message>
I made a few changes to enable me to work on my local machine
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -457,7 +457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
@@ -553,20 +553,40 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Starville Aingula</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>Subscribed</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Employed</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>John Kamau</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>18</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Subscribed</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>Employed</t>
         </is>

</xml_diff>

<commit_message>
I added a few changes to the main and added more information
</commit_message>
<xml_diff>
--- a/people.xlsx
+++ b/people.xlsx
@@ -457,7 +457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView showFormulas="0" showGridLines="1" showRowColHeaders="1" showZeros="1" rightToLeft="0" tabSelected="1" showOutlineSymbols="1" defaultGridColor="1" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
@@ -553,20 +553,40 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>Starville Aingula</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="B5" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>Subscribed</t>
         </is>
       </c>
-      <c r="D5" t="inlineStr">
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>Employed</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Jake Opiyo</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>29</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Not Subscribed</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
         <is>
           <t>Employed</t>
         </is>

</xml_diff>